<commit_message>
- Implement cocina output process
</commit_message>
<xml_diff>
--- a/storage/macros/cocina/Ejemplo.xlsx
+++ b/storage/macros/cocina/Ejemplo.xlsx
@@ -1,55 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas\xampp\htdocs\localUnal\storage\macros\cocina\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
-    <sheet name="Seccion 1" sheetId="2" r:id="rId5"/>
-    <sheet name="Seccion 2" sheetId="3" r:id="rId6"/>
-    <sheet name="Seccion 3" sheetId="4" r:id="rId7"/>
-    <sheet name="Pedido" sheetId="5" r:id="rId8"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Seccion 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Seccion 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Seccion 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Pedido" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
-    <t>5,00</t>
+    <t>1</t>
   </si>
   <si>
-    <t>3,50</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>pedidoID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -60,28 +53,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -371,48 +373,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="18" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>500</v>
+      </c>
+      <c r="B1">
+        <v>500</v>
+      </c>
+      <c r="C1">
+        <v>350</v>
       </c>
       <c r="D1">
         <v>2</v>
@@ -433,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K1">
         <v>4</v>
@@ -448,10 +431,10 @@
         <v>0</v>
       </c>
       <c r="O1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q1">
         <v>1</v>
@@ -461,200 +444,137 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="6" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.10" bestFit="true" style="0"/>
+    <col min="1" max="1" width="9.109375" bestFit="1"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Fix bugs in macros
</commit_message>
<xml_diff>
--- a/storage/macros/cocina/Ejemplo.xlsx
+++ b/storage/macros/cocina/Ejemplo.xlsx
@@ -1,29 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas\xampp\htdocs\localUnal\storage\macros\cocina\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6096" activeTab="4"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Seccion 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Seccion 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Seccion 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Pedido" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Seccion 1" sheetId="2" r:id="rId5"/>
+    <sheet name="Seccion 2" sheetId="3" r:id="rId6"/>
+    <sheet name="Seccion 3" sheetId="4" r:id="rId7"/>
+    <sheet name="Pedido" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>1</t>
   </si>
@@ -31,7 +27,10 @@
     <t>2</t>
   </si>
   <si>
-    <t>-</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>pedidoID</t>
@@ -40,9 +39,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -53,37 +57,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -373,38 +368,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="18" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="2.285156" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18">
       <c r="A1">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="B1">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="C1">
         <v>350</v>
       </c>
       <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
         <v>2</v>
       </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
       <c r="F1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -416,22 +430,22 @@
         <v>2</v>
       </c>
       <c r="J1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>4</v>
+      </c>
+      <c r="M1">
         <v>3</v>
       </c>
-      <c r="K1">
+      <c r="N1">
         <v>4</v>
       </c>
-      <c r="L1">
-        <v>3</v>
-      </c>
-      <c r="M1">
+      <c r="O1">
         <v>2</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>3</v>
       </c>
       <c r="P1" t="s">
         <v>0</v>
@@ -444,27 +458,110 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -472,109 +569,139 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="2.285156" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="2.285156" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1"/>
-  </cols>
-  <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.568848" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>